<commit_message>
Passing through updates due to swapping in 1prn and 3wi4
</commit_message>
<xml_diff>
--- a/IntRptsE-3.xlsx
+++ b/IntRptsE-3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghan/Documents/PhD/GitHubProjects/v6_2018_Network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88A25302-658C-C841-B8FC-A251FE704B50}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9929B0-8F27-9946-8C30-FCB4AAE64047}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="4960" windowWidth="38400" windowHeight="21140" xr2:uid="{ED293F74-59D3-5E48-9CAF-418D5E6D59CC}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{ED293F74-59D3-5E48-9CAF-418D5E6D59CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,15 +336,6 @@
     <t>379-451</t>
   </si>
   <si>
-    <t>3prn_A</t>
-  </si>
-  <si>
-    <t>130-261</t>
-  </si>
-  <si>
-    <t>163-289</t>
-  </si>
-  <si>
     <t>3qlb_A</t>
   </si>
   <si>
@@ -372,15 +363,6 @@
     <t>51-284</t>
   </si>
   <si>
-    <t>3wi5_A</t>
-  </si>
-  <si>
-    <t>126-277</t>
-  </si>
-  <si>
-    <t>160-312</t>
-  </si>
-  <si>
     <t>4aui_A</t>
   </si>
   <si>
@@ -780,12 +762,6 @@
     <t>(432)</t>
   </si>
   <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>(312)</t>
-  </si>
-  <si>
     <t>139</t>
   </si>
   <si>
@@ -928,6 +904,30 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>1prn_A</t>
+  </si>
+  <si>
+    <t>131-261</t>
+  </si>
+  <si>
+    <t>164-289</t>
+  </si>
+  <si>
+    <t>3wi4_A</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>128-278</t>
+  </si>
+  <si>
+    <t>162-313</t>
+  </si>
+  <si>
+    <t>(313)</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1299,34 +1299,34 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F1" t="s">
-        <v>296</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>1</v>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>101</v>
@@ -1364,40 +1364,42 @@
         <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="3">
         <v>99.5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>2.6999999999999998E-23</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>176.2</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>250</v>
-      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
@@ -1419,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>4</v>
@@ -1428,7 +1430,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>6</v>
@@ -1457,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>35</v>
@@ -1466,7 +1468,7 @@
         <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>6</v>
@@ -1495,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>84</v>
@@ -1504,7 +1506,7 @@
         <v>85</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>6</v>
@@ -1514,40 +1516,40 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="3">
         <v>99.4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>3.5999999999999999E-21</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>152.4</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1556,7 +1558,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C8">
         <v>99.4</v>
@@ -1571,16 +1573,16 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>6</v>
@@ -1590,116 +1592,116 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3">
         <v>99.5</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>1.1E-22</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>168.3</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="I9" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="3">
         <v>99.5</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>6.6000000000000004E-23</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>166.2</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="3">
         <v>99.5</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>4.3000000000000004E-22</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>161.4</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1723,16 +1725,16 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>10</v>
@@ -1761,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>18</v>
@@ -1770,7 +1772,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>20</v>
@@ -1799,16 +1801,16 @@
         <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>10</v>
@@ -1837,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>41</v>
@@ -1846,7 +1848,7 @@
         <v>42</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>10</v>
@@ -1875,16 +1877,16 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>10</v>
@@ -1913,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>56</v>
@@ -1922,7 +1924,7 @@
         <v>57</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>20</v>
@@ -1936,7 +1938,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C18">
         <v>91.3</v>
@@ -1951,16 +1953,16 @@
         <v>0</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>10</v>
@@ -1974,7 +1976,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C19">
         <v>82.8</v>
@@ -1989,16 +1991,16 @@
         <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>20</v>
@@ -2027,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>30</v>
@@ -2036,7 +2038,7 @@
         <v>31</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>32</v>
@@ -2065,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>51</v>
@@ -2074,7 +2076,7 @@
         <v>52</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>53</v>
@@ -2103,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>71</v>
@@ -2112,7 +2114,7 @@
         <v>72</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>73</v>
@@ -2141,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>95</v>
@@ -2150,7 +2152,7 @@
         <v>96</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>32</v>
@@ -2164,7 +2166,7 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C24">
         <v>94.4</v>
@@ -2179,16 +2181,16 @@
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>32</v>
@@ -2198,41 +2200,41 @@
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="3">
         <v>92.9</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="4">
         <v>3.7E-7</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>48.2</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="K25" s="2" t="s">
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L25" t="s">
-        <v>130</v>
+      <c r="L25" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2240,7 +2242,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C26">
         <v>76.599999999999994</v>
@@ -2255,22 +2257,22 @@
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="L26" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2293,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>25</v>
@@ -2302,7 +2304,7 @@
         <v>26</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>27</v>
@@ -2331,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>59</v>
@@ -2340,7 +2342,7 @@
         <v>60</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>21</v>
@@ -2369,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>76</v>
@@ -2378,7 +2380,7 @@
         <v>77</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>78</v>
@@ -2407,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>81</v>
@@ -2416,7 +2418,7 @@
         <v>82</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>78</v>
@@ -2445,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>87</v>
@@ -2454,7 +2456,7 @@
         <v>88</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>27</v>
@@ -2464,268 +2466,268 @@
       </c>
     </row>
     <row r="32" spans="1:12" s="3" customFormat="1">
-      <c r="A32" s="3">
+      <c r="A32">
         <v>16</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>97.5</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="1">
         <v>6.5000000000000002E-12</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>81.3</v>
       </c>
-      <c r="F32" s="3">
-        <v>0</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="H32" s="5" t="s">
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="K32" s="5" t="s">
+      <c r="J32" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="3" customFormat="1">
-      <c r="A33" s="3">
+      <c r="A33">
         <v>16</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" t="s">
+        <v>293</v>
+      </c>
+      <c r="C33">
+        <v>98.3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.3E-14</v>
+      </c>
+      <c r="E33">
+        <v>97.2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="3" customFormat="1">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C34">
         <v>97.4</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D34" s="1">
         <v>1.6E-11</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E34">
         <v>80.400000000000006</v>
       </c>
-      <c r="F33" s="3">
-        <v>0</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H33" s="5" t="s">
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J34" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="3" customFormat="1">
+      <c r="A35">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35">
+        <v>97.2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4.1000000000000001E-11</v>
+      </c>
+      <c r="E35">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="H35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="3" customFormat="1">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <v>97.3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2.2000000000000002E-11</v>
+      </c>
+      <c r="E36">
+        <v>79.7</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="L36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="3" customFormat="1">
-      <c r="A34" s="3">
+    <row r="37" spans="1:12" s="3" customFormat="1">
+      <c r="A37">
         <v>16</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="3">
-        <v>97.2</v>
-      </c>
-      <c r="D34" s="4">
-        <v>4.1000000000000001E-11</v>
-      </c>
-      <c r="E34" s="3">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="3" customFormat="1">
-      <c r="A35" s="3">
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <v>96.3</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.5E-9</v>
+      </c>
+      <c r="E37">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="3" customFormat="1">
+      <c r="A38">
         <v>16</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="3">
-        <v>97.3</v>
-      </c>
-      <c r="D35" s="4">
-        <v>2.2000000000000002E-11</v>
-      </c>
-      <c r="E35" s="3">
-        <v>79.7</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="K35" s="5" t="s">
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38">
+        <v>97.1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6.2000000000000006E-11</v>
+      </c>
+      <c r="E38">
+        <v>76</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L35" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="3" customFormat="1">
-      <c r="A36" s="3">
-        <v>16</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="3">
-        <v>96.3</v>
-      </c>
-      <c r="D36" s="4">
-        <v>1.5E-9</v>
-      </c>
-      <c r="E36" s="3">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="3" customFormat="1">
-      <c r="A37" s="3">
-        <v>16</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="3">
-        <v>97.1</v>
-      </c>
-      <c r="D37" s="4">
-        <v>6.2000000000000006E-11</v>
-      </c>
-      <c r="E37" s="3">
-        <v>76</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="3" customFormat="1">
-      <c r="A38" s="3">
-        <v>16</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="3">
-        <v>98.3</v>
-      </c>
-      <c r="D38" s="4">
-        <v>2.3E-14</v>
-      </c>
-      <c r="E38" s="3">
-        <v>96.1</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" s="3" t="s">
+      <c r="L38" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2734,31 +2736,31 @@
         <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>115</v>
+        <v>296</v>
       </c>
       <c r="C39" s="3">
-        <v>97.4</v>
+        <v>97.5</v>
       </c>
       <c r="D39" s="4">
-        <v>1.3E-11</v>
+        <v>4.9999999999999997E-12</v>
       </c>
       <c r="E39" s="3">
-        <v>79.099999999999994</v>
+        <v>82</v>
       </c>
       <c r="F39" s="3">
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>116</v>
+        <v>298</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>117</v>
+        <v>299</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>252</v>
+        <v>300</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>15</v>
@@ -2772,7 +2774,7 @@
         <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C40" s="3">
         <v>96.4</v>
@@ -2787,16 +2789,16 @@
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>15</v>
@@ -2806,37 +2808,38 @@
       </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>16</v>
       </c>
-      <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="3">
         <v>98</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="4">
         <v>1.9E-13</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="3">
         <v>108.4</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="L41">
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2845,7 +2848,7 @@
         <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C42" s="3">
         <v>97.1</v>
@@ -2860,16 +2863,16 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>15</v>
@@ -2879,105 +2882,109 @@
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>16</v>
       </c>
-      <c r="B43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43">
+      <c r="B43" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="3">
         <v>99.9</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="4">
         <v>1.6999999999999999E-32</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="3">
         <v>284</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>260</v>
-      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="3"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44">
+      <c r="A44" s="3">
         <v>16</v>
       </c>
-      <c r="B44" t="s">
-        <v>134</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="3">
         <v>87.3</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="4">
         <v>3.8E-6</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="3">
         <v>51.2</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>263</v>
-      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="K44" s="5"/>
+      <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45">
+      <c r="A45" s="3">
         <v>16</v>
       </c>
-      <c r="B45" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="3">
         <v>81</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="4">
         <v>1.2E-5</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="3">
         <v>44.7</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L45" t="s">
-        <v>159</v>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="3" customFormat="1">
@@ -2985,7 +2992,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C46" s="3">
         <v>96.8</v>
@@ -3000,16 +3007,16 @@
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>15</v>
@@ -3019,154 +3026,154 @@
       </c>
     </row>
     <row r="47" spans="1:12" s="3" customFormat="1">
-      <c r="A47" s="3">
+      <c r="A47">
         <v>16</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="3">
+      <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47">
         <v>97.1</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="1">
         <v>7.8000000000000002E-11</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47">
         <v>78.3</v>
       </c>
-      <c r="F47" s="3">
-        <v>0</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I47" s="5" t="s">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="3" customFormat="1">
+      <c r="A48">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
         <v>174</v>
       </c>
-      <c r="J47" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="K47" s="5" t="s">
+      <c r="C48">
+        <v>96.9</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2.0000000000000001E-10</v>
+      </c>
+      <c r="E48">
+        <v>73.7</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L47" s="3" t="s">
+      <c r="L48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="3" customFormat="1">
-      <c r="A48" s="3">
+    <row r="49" spans="1:12" s="3" customFormat="1">
+      <c r="A49">
         <v>16</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49">
+        <v>97</v>
+      </c>
+      <c r="D49" s="1">
+        <v>9.2000000000000005E-11</v>
+      </c>
+      <c r="E49">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="3" customFormat="1">
+      <c r="A50">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
         <v>180</v>
       </c>
-      <c r="C48" s="3">
-        <v>96.9</v>
-      </c>
-      <c r="D48" s="4">
-        <v>2.0000000000000001E-10</v>
-      </c>
-      <c r="E48" s="3">
-        <v>73.7</v>
-      </c>
-      <c r="F48" s="3">
-        <v>0</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="H48" s="5" t="s">
+      <c r="C50">
+        <v>96.7</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4.3999999999999998E-10</v>
+      </c>
+      <c r="E50">
+        <v>69.8</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I50" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="J48" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="K48" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L48" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="3" customFormat="1">
-      <c r="A49" s="3">
-        <v>16</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C49" s="3">
-        <v>97</v>
-      </c>
-      <c r="D49" s="4">
-        <v>9.2000000000000005E-11</v>
-      </c>
-      <c r="E49" s="3">
-        <v>73.900000000000006</v>
-      </c>
-      <c r="F49" s="3">
-        <v>0</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="K49" s="5" t="s">
+      <c r="J50" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L49" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="3" customFormat="1">
-      <c r="A50" s="3">
-        <v>16</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C50" s="3">
-        <v>96.7</v>
-      </c>
-      <c r="D50" s="4">
-        <v>4.3999999999999998E-10</v>
-      </c>
-      <c r="E50" s="3">
-        <v>69.8</v>
-      </c>
-      <c r="F50" s="3">
-        <v>0</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L50" s="3" t="s">
+      <c r="L50" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3190,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>90</v>
@@ -3199,7 +3206,7 @@
         <v>91</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>92</v>
@@ -3213,7 +3220,7 @@
         <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C52">
         <v>95.8</v>
@@ -3228,16 +3235,16 @@
         <v>0</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3245,7 +3252,7 @@
         <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C53">
         <v>78.400000000000006</v>
@@ -3260,22 +3267,22 @@
         <v>0</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L53" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3283,7 +3290,7 @@
         <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C54">
         <v>95.4</v>
@@ -3298,49 +3305,51 @@
         <v>0</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55">
+      <c r="A55" s="3">
         <v>26</v>
       </c>
-      <c r="B55" t="s">
-        <v>169</v>
-      </c>
-      <c r="C55">
+      <c r="B55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="3">
         <v>95.3</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="4">
         <v>2.0999999999999999E-8</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="3">
         <v>80.2</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>283</v>
-      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="K55" s="5"/>
+      <c r="L55" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:L56">

</xml_diff>